<commit_message>
Generador pdf y  Act BD
</commit_message>
<xml_diff>
--- a/DisBD.xlsx
+++ b/DisBD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maego\OneDrive\Documentos\UAdeC_Archivos ISC\Diseño y arquitectura de Software_S7_Ago_Dic_2023\Carpetas programas\Java\Parcial 2 Proyecto DSKT Ticket de turno_Mario Palacio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Web_Tiket_Turno\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562F6153-88D2-4077-84C0-65A9B67A84A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B6641A-189E-42DF-B10A-C0931C761D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{049A9011-596B-4021-8943-969E275BE614}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Administrador</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>Num_cita</t>
+  </si>
+  <si>
+    <t>Asuntos</t>
+  </si>
+  <si>
+    <t>Id_asunto</t>
+  </si>
+  <si>
+    <t>OTR</t>
   </si>
 </sst>
 </file>
@@ -535,7 +544,7 @@
   <dimension ref="C4:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,21 +607,34 @@
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="F11" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="L11" s="3"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="F13" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>